<commit_message>
Diary Entry for Aman Bhatia
</commit_message>
<xml_diff>
--- a/diaries/diary-AmanBhatia.xlsx
+++ b/diaries/diary-AmanBhatia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanbhatia/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E817E5-F8DB-3A46-BBE6-5942EB0138A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5105AB-0ACB-3E46-B044-D4DACAE48350}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="172">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -487,6 +487,72 @@
   </si>
   <si>
     <t>Some patterns like Factory are easy to search if proper naming conventions are followed, like SessionFactory</t>
+  </si>
+  <si>
+    <t>Learn new KEP and concepts</t>
+  </si>
+  <si>
+    <t>Learned new concepts and key expert practices. Also learnt from Eric and Michaels experience</t>
+  </si>
+  <si>
+    <t>Testing not only helps us in improving confidence and coverage of our code. It can also revela a lot of information about how the system works. And thus I learn't today that in addition to all the tehniwues for understanding the system, I could also use the test cases and try to decipher the system's working.</t>
+  </si>
+  <si>
+    <t>11:00 am - 12:30 pm</t>
+  </si>
+  <si>
+    <t>Find a second issue to work on and submit a pull request for approval</t>
+  </si>
+  <si>
+    <t>We identified a non trivial issue and submitted a pull request for it, which was later approved by Kaj</t>
+  </si>
+  <si>
+    <t>We picked this particular issue, since it was properly described and also becauseit dealt with an error during insertion(which is an important feature of h2 or any database for that matter)</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t>Could not attend the lecture as I wasn't feeling very well and didn't want to step out in a rainy kind of weather, readfrom a friend's notes</t>
+  </si>
+  <si>
+    <t>Read from a friends notes</t>
+  </si>
+  <si>
+    <t>Fix the issue and submit a pull request for it</t>
+  </si>
+  <si>
+    <t>We figured out where in the code, the issue lied, and submitted a pull request for the issue</t>
+  </si>
+  <si>
+    <t>Our familiarity with h2 database , helped us in understanding where the issue lied. We put breakpoints at specific places(which we knew from pur previous understanding) and were able to pin point the error's location by going through the flow. System understanding indeed helps when you try to add in new changes or fix old code.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good, since we were excited after solving this bug, </t>
+  </si>
+  <si>
+    <t>Identify three interesting test cases and document those</t>
+  </si>
+  <si>
+    <t>We understood that the test suite in this project is not conventional and the unit test are not written using Junit. We also learnt that benchmarking is important, if you want to find out bottlenecks in your application and improve runtime and space complexity</t>
+  </si>
+  <si>
+    <t>Went through test cases, identified three interesting ones and documented the same</t>
+  </si>
+  <si>
+    <t>9 pm - 11 pm</t>
+  </si>
+  <si>
+    <t>Work on third part of the hoework</t>
+  </si>
+  <si>
+    <t>Create three new test cases and finsih the report</t>
+  </si>
+  <si>
+    <t>We were surprised to see that even though this is a complicated project, there were so many edge cases left uncovered like referential integrity constraint violation error</t>
+  </si>
+  <si>
+    <t>Feeling good after finishing the reports.</t>
   </si>
 </sst>
 </file>
@@ -987,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="156" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="156" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1749,59 +1815,141 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
+    <row r="38" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A38" s="10">
+        <v>43895</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A39" s="10">
+        <v>43898</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A40" s="10">
+        <v>43902</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>159</v>
+      </c>
       <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8"/>
+      <c r="G40" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="A41" s="10">
+        <v>43903</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A42" s="10">
+        <v>43904</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A43" s="10">
+        <v>43905</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>

</xml_diff>